<commit_message>
añade DIAS_EXCLUIR, quita días de los posibles laborables
oculta lista_dias ya que no se usa, pero se deja por ser útl para desarrollo
</commit_message>
<xml_diff>
--- a/fichero_prueba_relleno.xlsx
+++ b/fichero_prueba_relleno.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="0" windowWidth="0" xWindow="0" yWindow="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="IGNACIO ANTON HERNANDEZ" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcCompleted="0" calcId="191028" calcOnSave="0" concurrentCalc="0" fullCalcOnLoad="1" iterateCount="0" refMode="R1C1"/>
+  <calcPr calcId="191028" fullCalcOnLoad="1" refMode="R1C1" iterateCount="0" calcCompleted="0" calcOnSave="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -183,49 +183,49 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyProtection="1" borderId="1" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="7" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="8" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="9" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="3" fillId="9" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -606,30 +606,30 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="8" width="12.5703125"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="8" width="116.7109375"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="8" width="113.5703125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="8" width="68.42578125"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="8" width="110.42578125"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="8" width="65.5703125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="8" width="83.28515625"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="8" width="99.140625"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="8" width="124"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="8" width="93.5703125"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="8" width="79.7109375"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="8" width="60.85546875"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" style="8" width="114.85546875"/>
-    <col bestFit="1" customWidth="1" max="14" min="14" style="8" width="64.42578125"/>
-    <col bestFit="1" customWidth="1" max="15" min="15" style="8" width="19.28515625"/>
-    <col bestFit="1" customWidth="1" max="16" min="16" style="8" width="11.5703125"/>
-    <col bestFit="1" customWidth="1" max="17" min="17" style="8" width="21.140625"/>
-    <col bestFit="1" customWidth="1" max="18" min="18" style="8" width="7.85546875"/>
-    <col bestFit="1" customWidth="1" max="20" min="20" style="8" width="111.28515625"/>
-    <col bestFit="1" customWidth="1" max="21" min="21" style="8" width="7.85546875"/>
-    <col customWidth="1" hidden="1" max="151" min="151" style="8" width="8"/>
+    <col width="12.5703125" bestFit="1" customWidth="1" style="8" min="1" max="1"/>
+    <col width="116.7109375" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="113.5703125" bestFit="1" customWidth="1" style="8" min="3" max="3"/>
+    <col width="68.42578125" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
+    <col width="110.42578125" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
+    <col width="65.5703125" bestFit="1" customWidth="1" style="8" min="6" max="6"/>
+    <col width="83.28515625" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
+    <col width="99.140625" bestFit="1" customWidth="1" style="8" min="8" max="8"/>
+    <col width="124" bestFit="1" customWidth="1" style="8" min="9" max="9"/>
+    <col width="93.5703125" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
+    <col width="79.7109375" bestFit="1" customWidth="1" style="8" min="11" max="11"/>
+    <col width="60.85546875" bestFit="1" customWidth="1" style="8" min="12" max="12"/>
+    <col width="114.85546875" bestFit="1" customWidth="1" style="8" min="13" max="13"/>
+    <col width="64.42578125" bestFit="1" customWidth="1" style="8" min="14" max="14"/>
+    <col width="19.28515625" bestFit="1" customWidth="1" style="8" min="15" max="15"/>
+    <col width="11.5703125" bestFit="1" customWidth="1" style="8" min="16" max="16"/>
+    <col width="21.140625" bestFit="1" customWidth="1" style="8" min="17" max="17"/>
+    <col width="7.85546875" bestFit="1" customWidth="1" style="8" min="18" max="18"/>
+    <col width="111.28515625" bestFit="1" customWidth="1" style="8" min="20" max="20"/>
+    <col width="7.85546875" bestFit="1" customWidth="1" style="8" min="21" max="21"/>
+    <col hidden="1" width="8" customWidth="1" style="8" min="151" max="151"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="27.6" r="1" s="8">
+    <row r="1" ht="27.6" customHeight="1" s="8">
       <c r="A1" t="inlineStr"/>
       <c r="B1" s="7" t="inlineStr">
         <is>
@@ -2977,7 +2977,7 @@
         <v>0</v>
       </c>
       <c r="N37" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O37" s="3" t="n">
         <v>0</v>
@@ -3499,7 +3499,7 @@
         <v>0</v>
       </c>
       <c r="K46" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L46" s="3" t="n">
         <v>0</v>
@@ -3508,7 +3508,7 @@
         <v>0</v>
       </c>
       <c r="N46" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O46" s="3" t="n">
         <v>0</v>
@@ -3974,7 +3974,7 @@
         <v>0.5</v>
       </c>
       <c r="L54" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M54" s="3" t="n">
         <v>0.5</v>
@@ -4599,16 +4599,16 @@
         <v>0</v>
       </c>
       <c r="D65" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E65" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F65" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G65" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H65" s="3" t="n">
         <v>0</v>
@@ -4620,7 +4620,7 @@
         <v>0</v>
       </c>
       <c r="K65" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L65" s="3" t="n">
         <v>0</v>
@@ -4717,7 +4717,7 @@
         <v>0</v>
       </c>
       <c r="D67" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E67" s="3" t="n">
         <v>0</v>
@@ -4782,7 +4782,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G68" s="3" t="n">
         <v>0</v>
@@ -4797,10 +4797,10 @@
         <v>0</v>
       </c>
       <c r="K68" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L68" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M68" s="3" t="n">
         <v>0</v>
@@ -5018,10 +5018,10 @@
         <v>0</v>
       </c>
       <c r="F72" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G72" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H72" s="3" t="n">
         <v>0</v>
@@ -5033,13 +5033,13 @@
         <v>0</v>
       </c>
       <c r="K72" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L72" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M72" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N72" s="3" t="n">
         <v>0</v>
@@ -5077,7 +5077,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G73" s="3" t="n">
         <v>0</v>
@@ -5133,7 +5133,7 @@
         <v>0</v>
       </c>
       <c r="E74" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F74" s="3" t="n">
         <v>0</v>
@@ -5210,16 +5210,16 @@
         <v>0</v>
       </c>
       <c r="K75" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L75" s="3" t="n">
         <v>0</v>
       </c>
       <c r="M75" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N75" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O75" s="3" t="n">
         <v>0</v>
@@ -5269,13 +5269,13 @@
         <v>0</v>
       </c>
       <c r="K76" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L76" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M76" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N76" s="3" t="n">
         <v>0.5</v>
@@ -5446,7 +5446,7 @@
         <v>0</v>
       </c>
       <c r="K79" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L79" s="3" t="n">
         <v>0</v>
@@ -5487,7 +5487,7 @@
         <v>0</v>
       </c>
       <c r="E80" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F80" s="3" t="n">
         <v>0</v>
@@ -5505,7 +5505,7 @@
         <v>0</v>
       </c>
       <c r="K80" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L80" s="3" t="n">
         <v>0</v>
@@ -5546,7 +5546,7 @@
         <v>0</v>
       </c>
       <c r="E81" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F81" s="3" t="n">
         <v>0</v>
@@ -5608,7 +5608,7 @@
         <v>0</v>
       </c>
       <c r="F82" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G82" s="3" t="n">
         <v>0</v>
@@ -5623,10 +5623,10 @@
         <v>0</v>
       </c>
       <c r="K82" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L82" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M82" s="3" t="n">
         <v>0</v>
@@ -5667,10 +5667,10 @@
         <v>0</v>
       </c>
       <c r="F83" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G83" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H83" s="3" t="n">
         <v>0</v>
@@ -5682,13 +5682,13 @@
         <v>0</v>
       </c>
       <c r="K83" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L83" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M83" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N83" s="3" t="n">
         <v>0</v>
@@ -5921,13 +5921,13 @@
         <v>0.5</v>
       </c>
       <c r="L87" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M87" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N87" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O87" s="3" t="n">
         <v>0</v>
@@ -5962,7 +5962,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G88" s="3" t="n">
         <v>0</v>
@@ -5977,7 +5977,7 @@
         <v>0</v>
       </c>
       <c r="K88" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L88" s="3" t="n">
         <v>0</v>
@@ -6021,10 +6021,10 @@
         <v>0</v>
       </c>
       <c r="F89" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G89" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H89" s="3" t="n">
         <v>0</v>
@@ -6036,7 +6036,7 @@
         <v>0</v>
       </c>
       <c r="K89" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L89" s="3" t="n">
         <v>0</v>
@@ -6316,7 +6316,7 @@
         <v>0</v>
       </c>
       <c r="F94" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G94" s="3" t="n">
         <v>0</v>
@@ -6331,10 +6331,10 @@
         <v>0</v>
       </c>
       <c r="K94" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L94" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M94" s="3" t="n">
         <v>0</v>
@@ -6372,10 +6372,10 @@
         <v>0</v>
       </c>
       <c r="E95" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F95" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G95" s="3" t="n">
         <v>0</v>
@@ -6431,13 +6431,13 @@
         <v>0</v>
       </c>
       <c r="E96" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F96" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G96" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H96" s="3" t="n">
         <v>0</v>
@@ -6508,7 +6508,7 @@
         <v>0</v>
       </c>
       <c r="K97" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L97" s="3" t="n">
         <v>0</v>
@@ -6517,7 +6517,7 @@
         <v>0</v>
       </c>
       <c r="N97" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O97" s="3" t="n">
         <v>0</v>
@@ -6685,16 +6685,16 @@
         <v>0</v>
       </c>
       <c r="K100" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L100" s="3" t="n">
         <v>0</v>
       </c>
       <c r="M100" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N100" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O100" s="3" t="n">
         <v>0</v>
@@ -7195,7 +7195,7 @@
         <v>0</v>
       </c>
       <c r="D109" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E109" s="3" t="n">
         <v>0</v>
@@ -7257,13 +7257,13 @@
         <v>0</v>
       </c>
       <c r="E110" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F110" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G110" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H110" s="3" t="n">
         <v>0</v>
@@ -7319,7 +7319,7 @@
         <v>0</v>
       </c>
       <c r="F111" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G111" s="3" t="n">
         <v>0</v>
@@ -7555,10 +7555,10 @@
         <v>0</v>
       </c>
       <c r="F115" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G115" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H115" s="3" t="n">
         <v>0</v>
@@ -7570,7 +7570,7 @@
         <v>0</v>
       </c>
       <c r="K115" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L115" s="3" t="n">
         <v>0</v>
@@ -8051,7 +8051,7 @@
         <v>0</v>
       </c>
       <c r="N123" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O123" s="3" t="n">
         <v>0</v>
@@ -8101,7 +8101,7 @@
         <v>0</v>
       </c>
       <c r="K124" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L124" s="3" t="n">
         <v>0</v>
@@ -8110,7 +8110,7 @@
         <v>0</v>
       </c>
       <c r="N124" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O124" s="3" t="n">
         <v>0</v>
@@ -8316,7 +8316,7 @@
         <v>0</v>
       </c>
       <c r="D128" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E128" s="3" t="n">
         <v>0</v>
@@ -8375,7 +8375,7 @@
         <v>0</v>
       </c>
       <c r="D129" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E129" s="3" t="n">
         <v>0</v>
@@ -8396,7 +8396,7 @@
         <v>0</v>
       </c>
       <c r="K129" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L129" s="3" t="n">
         <v>0</v>
@@ -8455,7 +8455,7 @@
         <v>0</v>
       </c>
       <c r="K130" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L130" s="3" t="n">
         <v>0</v>
@@ -9142,13 +9142,13 @@
         <v>0</v>
       </c>
       <c r="D142" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E142" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F142" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G142" s="3" t="n">
         <v>0</v>
@@ -9204,7 +9204,7 @@
         <v>0</v>
       </c>
       <c r="E143" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F143" s="3" t="n">
         <v>0.5</v>
@@ -9222,7 +9222,7 @@
         <v>0</v>
       </c>
       <c r="K143" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L143" s="3" t="n">
         <v>0</v>
@@ -9260,13 +9260,13 @@
         <v>0</v>
       </c>
       <c r="D144" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E144" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F144" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G144" s="3" t="n">
         <v>0</v>
@@ -9620,10 +9620,10 @@
         <v>0</v>
       </c>
       <c r="F150" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G150" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H150" s="3" t="n">
         <v>0</v>
@@ -9635,13 +9635,13 @@
         <v>0</v>
       </c>
       <c r="K150" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L150" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M150" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N150" s="3" t="n">
         <v>0</v>
@@ -9679,7 +9679,7 @@
         <v>0</v>
       </c>
       <c r="F151" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G151" s="3" t="n">
         <v>0</v>
@@ -9732,13 +9732,13 @@
         <v>0</v>
       </c>
       <c r="D152" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E152" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F152" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G152" s="3" t="n">
         <v>0</v>
@@ -9968,7 +9968,7 @@
         <v>0</v>
       </c>
       <c r="D156" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E156" s="3" t="n">
         <v>0.5</v>
@@ -9977,7 +9977,7 @@
         <v>0.5</v>
       </c>
       <c r="G156" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H156" s="3" t="n">
         <v>0</v>
@@ -10033,7 +10033,7 @@
         <v>0</v>
       </c>
       <c r="F157" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G157" s="3" t="n">
         <v>0</v>
@@ -10048,7 +10048,7 @@
         <v>0</v>
       </c>
       <c r="K157" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L157" s="3" t="n">
         <v>0</v>
@@ -10086,7 +10086,7 @@
         <v>0</v>
       </c>
       <c r="D158" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E158" s="3" t="n">
         <v>0</v>
@@ -10225,7 +10225,7 @@
         <v>0</v>
       </c>
       <c r="K160" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L160" s="3" t="n">
         <v>0</v>
@@ -10387,7 +10387,7 @@
         <v>0</v>
       </c>
       <c r="F163" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G163" s="3" t="n">
         <v>0</v>
@@ -10502,13 +10502,13 @@
         <v>0</v>
       </c>
       <c r="E165" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F165" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G165" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H165" s="3" t="n">
         <v>0</v>
@@ -10800,7 +10800,7 @@
         <v>0</v>
       </c>
       <c r="F170" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G170" s="3" t="n">
         <v>0</v>
@@ -10821,7 +10821,7 @@
         <v>0.5</v>
       </c>
       <c r="M170" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N170" s="3" t="n">
         <v>0</v>
@@ -10853,13 +10853,13 @@
         <v>0</v>
       </c>
       <c r="D171" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E171" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F171" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G171" s="3" t="n">
         <v>0</v>
@@ -10918,7 +10918,7 @@
         <v>0</v>
       </c>
       <c r="F172" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G172" s="3" t="n">
         <v>0</v>
@@ -10971,13 +10971,13 @@
         <v>0</v>
       </c>
       <c r="D173" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E173" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F173" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G173" s="3" t="n">
         <v>0</v>
@@ -11030,7 +11030,7 @@
         <v>0</v>
       </c>
       <c r="D174" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E174" s="3" t="n">
         <v>0</v>
@@ -11213,10 +11213,10 @@
         <v>0</v>
       </c>
       <c r="F177" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G177" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H177" s="3" t="n">
         <v>0</v>
@@ -11228,7 +11228,7 @@
         <v>0</v>
       </c>
       <c r="K177" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L177" s="3" t="n">
         <v>0</v>
@@ -11443,7 +11443,7 @@
         <v>0</v>
       </c>
       <c r="D181" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E181" s="3" t="n">
         <v>0</v>
@@ -11626,10 +11626,10 @@
         <v>0</v>
       </c>
       <c r="F184" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G184" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H184" s="3" t="n">
         <v>0</v>
@@ -11641,7 +11641,7 @@
         <v>0</v>
       </c>
       <c r="K184" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L184" s="3" t="n">
         <v>0</v>
@@ -11797,13 +11797,13 @@
         <v>0</v>
       </c>
       <c r="D187" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E187" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F187" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G187" s="3" t="n">
         <v>0</v>
@@ -11856,7 +11856,7 @@
         <v>0</v>
       </c>
       <c r="D188" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E188" s="3" t="n">
         <v>0</v>
@@ -12113,13 +12113,13 @@
         <v>0</v>
       </c>
       <c r="K192" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L192" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M192" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N192" s="3" t="n">
         <v>0</v>
@@ -12210,13 +12210,13 @@
         <v>0</v>
       </c>
       <c r="D194" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E194" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F194" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G194" s="3" t="n">
         <v>0</v>
@@ -12275,7 +12275,7 @@
         <v>0</v>
       </c>
       <c r="F195" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G195" s="3" t="n">
         <v>0</v>
@@ -12452,10 +12452,10 @@
         <v>0</v>
       </c>
       <c r="F198" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G198" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H198" s="3" t="n">
         <v>0</v>
@@ -12467,7 +12467,7 @@
         <v>0</v>
       </c>
       <c r="K198" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L198" s="3" t="n">
         <v>0</v>
@@ -12511,10 +12511,10 @@
         <v>0</v>
       </c>
       <c r="F199" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G199" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H199" s="3" t="n">
         <v>0</v>
@@ -12526,7 +12526,7 @@
         <v>0</v>
       </c>
       <c r="K199" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L199" s="3" t="n">
         <v>0</v>
@@ -12570,10 +12570,10 @@
         <v>0</v>
       </c>
       <c r="F200" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G200" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H200" s="3" t="n">
         <v>0</v>
@@ -12585,7 +12585,7 @@
         <v>0</v>
       </c>
       <c r="K200" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L200" s="3" t="n">
         <v>0</v>
@@ -12629,10 +12629,10 @@
         <v>0</v>
       </c>
       <c r="F201" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G201" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H201" s="3" t="n">
         <v>0</v>
@@ -12644,7 +12644,7 @@
         <v>0</v>
       </c>
       <c r="K201" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L201" s="3" t="n">
         <v>0</v>
@@ -12682,7 +12682,7 @@
         <v>0</v>
       </c>
       <c r="D202" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E202" s="3" t="n">
         <v>0</v>
@@ -12880,7 +12880,7 @@
         <v>0</v>
       </c>
       <c r="K205" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L205" s="3" t="n">
         <v>0</v>
@@ -13042,7 +13042,7 @@
         <v>0</v>
       </c>
       <c r="F208" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G208" s="3" t="n">
         <v>0</v>
@@ -13098,7 +13098,7 @@
         <v>0</v>
       </c>
       <c r="E209" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F209" s="3" t="n">
         <v>0</v>
@@ -13278,10 +13278,10 @@
         <v>0</v>
       </c>
       <c r="F212" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G212" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H212" s="3" t="n">
         <v>0</v>
@@ -13293,7 +13293,7 @@
         <v>0</v>
       </c>
       <c r="K212" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L212" s="3" t="n">
         <v>0</v>
@@ -13390,7 +13390,7 @@
         <v>0</v>
       </c>
       <c r="D214" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E214" s="3" t="n">
         <v>0</v>
@@ -13508,7 +13508,7 @@
         <v>0</v>
       </c>
       <c r="D216" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E216" s="3" t="n">
         <v>0</v>
@@ -15402,7 +15402,7 @@
         <v>0</v>
       </c>
       <c r="F248" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G248" s="3" t="n">
         <v>0</v>
@@ -15461,10 +15461,10 @@
         <v>0</v>
       </c>
       <c r="F249" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G249" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H249" s="3" t="n">
         <v>0</v>
@@ -15476,13 +15476,13 @@
         <v>0</v>
       </c>
       <c r="K249" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L249" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M249" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N249" s="3" t="n">
         <v>0</v>
@@ -15579,7 +15579,7 @@
         <v>0</v>
       </c>
       <c r="F251" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G251" s="3" t="n">
         <v>0</v>
@@ -15756,7 +15756,7 @@
         <v>0</v>
       </c>
       <c r="F254" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G254" s="3" t="n">
         <v>0</v>
@@ -15830,7 +15830,7 @@
         <v>0</v>
       </c>
       <c r="K255" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L255" s="3" t="n">
         <v>0</v>
@@ -15839,7 +15839,7 @@
         <v>0</v>
       </c>
       <c r="N255" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O255" s="3" t="n">
         <v>0</v>
@@ -15992,7 +15992,7 @@
         <v>0</v>
       </c>
       <c r="F258" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G258" s="3" t="n">
         <v>0</v>
@@ -16252,7 +16252,7 @@
         <v>0</v>
       </c>
       <c r="N262" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O262" s="3" t="n">
         <v>0</v>
@@ -16361,7 +16361,7 @@
         <v>0</v>
       </c>
       <c r="K264" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L264" s="3" t="n">
         <v>0</v>
@@ -16370,7 +16370,7 @@
         <v>0</v>
       </c>
       <c r="N264" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O264" s="3" t="n">
         <v>0</v>
@@ -16405,7 +16405,7 @@
         <v>0</v>
       </c>
       <c r="F265" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G265" s="3" t="n">
         <v>0</v>
@@ -16818,7 +16818,7 @@
         <v>0</v>
       </c>
       <c r="F272" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G272" s="3" t="n">
         <v>0</v>
@@ -16833,7 +16833,7 @@
         <v>0</v>
       </c>
       <c r="K272" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L272" s="3" t="n">
         <v>0</v>
@@ -17048,13 +17048,13 @@
         <v>0</v>
       </c>
       <c r="D276" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E276" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F276" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G276" s="3" t="n">
         <v>0</v>
@@ -17225,13 +17225,13 @@
         <v>0</v>
       </c>
       <c r="D279" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E279" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F279" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G279" s="3" t="n">
         <v>0</v>
@@ -17461,13 +17461,13 @@
         <v>0</v>
       </c>
       <c r="D283" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E283" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F283" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G283" s="3" t="n">
         <v>0</v>
@@ -17482,13 +17482,13 @@
         <v>0</v>
       </c>
       <c r="K283" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L283" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M283" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N283" s="3" t="n">
         <v>0</v>
@@ -17659,7 +17659,7 @@
         <v>0</v>
       </c>
       <c r="K286" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L286" s="3" t="n">
         <v>0</v>
@@ -17874,13 +17874,13 @@
         <v>0</v>
       </c>
       <c r="D290" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E290" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F290" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G290" s="3" t="n">
         <v>0</v>
@@ -17963,7 +17963,7 @@
         <v>0</v>
       </c>
       <c r="N291" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O291" s="3" t="n">
         <v>0</v>
@@ -18051,16 +18051,16 @@
         <v>0</v>
       </c>
       <c r="D293" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E293" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F293" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G293" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H293" s="3" t="n">
         <v>0</v>
@@ -18075,13 +18075,13 @@
         <v>0.5</v>
       </c>
       <c r="L293" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M293" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N293" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O293" s="3" t="n">
         <v>0</v>
@@ -18346,13 +18346,13 @@
         <v>0</v>
       </c>
       <c r="D298" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E298" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F298" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G298" s="3" t="n">
         <v>0</v>
@@ -18376,7 +18376,7 @@
         <v>0</v>
       </c>
       <c r="N298" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O298" s="3" t="n">
         <v>0</v>
@@ -18426,7 +18426,7 @@
         <v>0</v>
       </c>
       <c r="K299" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L299" s="3" t="n">
         <v>0</v>
@@ -18435,7 +18435,7 @@
         <v>0</v>
       </c>
       <c r="N299" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O299" s="3" t="n">
         <v>0</v>
@@ -18641,13 +18641,13 @@
         <v>0</v>
       </c>
       <c r="D303" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E303" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F303" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G303" s="3" t="n">
         <v>0</v>
@@ -18700,13 +18700,13 @@
         <v>0</v>
       </c>
       <c r="D304" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E304" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F304" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G304" s="3" t="n">
         <v>0</v>
@@ -18818,10 +18818,10 @@
         <v>0</v>
       </c>
       <c r="D306" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E306" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F306" s="3" t="n">
         <v>0.5</v>
@@ -18839,10 +18839,10 @@
         <v>0</v>
       </c>
       <c r="K306" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L306" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M306" s="3" t="n">
         <v>0</v>
@@ -19172,10 +19172,10 @@
         <v>0</v>
       </c>
       <c r="D312" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E312" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F312" s="3" t="n">
         <v>0.5</v>
@@ -19526,13 +19526,13 @@
         <v>0</v>
       </c>
       <c r="D318" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E318" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F318" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G318" s="3" t="n">
         <v>0</v>
@@ -19547,7 +19547,7 @@
         <v>0</v>
       </c>
       <c r="K318" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L318" s="3" t="n">
         <v>0</v>
@@ -19556,7 +19556,7 @@
         <v>0</v>
       </c>
       <c r="N318" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O318" s="3" t="n">
         <v>0</v>
@@ -19591,10 +19591,10 @@
         <v>0</v>
       </c>
       <c r="F319" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G319" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H319" s="3" t="n">
         <v>0</v>
@@ -19606,16 +19606,16 @@
         <v>0</v>
       </c>
       <c r="K319" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L319" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M319" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N319" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O319" s="3" t="n">
         <v>0</v>
@@ -19880,7 +19880,7 @@
         <v>0</v>
       </c>
       <c r="D324" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E324" s="3" t="n">
         <v>0.5</v>
@@ -19889,7 +19889,7 @@
         <v>0.5</v>
       </c>
       <c r="G324" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H324" s="3" t="n">
         <v>0</v>
@@ -20122,7 +20122,7 @@
         <v>0</v>
       </c>
       <c r="F328" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G328" s="3" t="n">
         <v>0</v>
@@ -20137,7 +20137,7 @@
         <v>0</v>
       </c>
       <c r="K328" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L328" s="3" t="n">
         <v>0</v>
@@ -20373,7 +20373,7 @@
         <v>0</v>
       </c>
       <c r="K332" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L332" s="3" t="n">
         <v>0</v>
@@ -20417,10 +20417,10 @@
         <v>0</v>
       </c>
       <c r="F333" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G333" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H333" s="3" t="n">
         <v>0</v>
@@ -20435,10 +20435,10 @@
         <v>0.5</v>
       </c>
       <c r="L333" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M333" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N333" s="3" t="n">
         <v>0</v>
@@ -20470,10 +20470,10 @@
         <v>0</v>
       </c>
       <c r="D334" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E334" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F334" s="3" t="n">
         <v>0.5</v>
@@ -20494,10 +20494,10 @@
         <v>0.5</v>
       </c>
       <c r="L334" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M334" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N334" s="3" t="n">
         <v>0</v>
@@ -20529,7 +20529,7 @@
         <v>0</v>
       </c>
       <c r="D335" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E335" s="3" t="n">
         <v>0</v>
@@ -20550,7 +20550,7 @@
         <v>0</v>
       </c>
       <c r="K335" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L335" s="3" t="n">
         <v>0</v>
@@ -20827,7 +20827,7 @@
         <v>0</v>
       </c>
       <c r="E340" s="3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F340" s="3" t="n">
         <v>0.5</v>
@@ -20883,16 +20883,16 @@
         <v>0</v>
       </c>
       <c r="D341" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E341" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F341" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G341" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H341" s="3" t="n">
         <v>0</v>
@@ -20904,16 +20904,16 @@
         <v>0</v>
       </c>
       <c r="K341" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L341" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M341" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N341" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O341" s="3" t="n">
         <v>0</v>
@@ -21240,13 +21240,13 @@
         <v>0</v>
       </c>
       <c r="E347" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F347" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G347" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H347" s="3" t="n">
         <v>0</v>
@@ -21709,10 +21709,10 @@
         <v>0</v>
       </c>
       <c r="D355" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E355" s="3" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F355" s="3" t="n">
         <v>0.5</v>
@@ -22593,12 +22593,12 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="1" password="EA46" pivotTables="1" scenarios="1" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="1" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="EA46"/>
   <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="B2:Q2"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>